<commit_message>
Add config model and core app, and load from source functionality
</commit_message>
<xml_diff>
--- a/server/app/tests/files/test_data.xlsx
+++ b/server/app/tests/files/test_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Shortcut" sheetId="1" state="visible" r:id="rId3"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="127">
   <si>
     <t xml:space="preserve">application_name</t>
   </si>
@@ -55,6 +55,285 @@
     <t xml:space="preserve">category</t>
   </si>
   <si>
+    <t xml:space="preserve">Google Chrome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open Dev Tools Console</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd + Opt + J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beginner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Google Sheets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit Selected Cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show Keyboard Shortcuts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd + /</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See Keyboard Shortcuts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search the Menus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opt + /</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tool Finder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MacOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch Between Open Apps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd + Tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spotlight Search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd + Space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global search through all files, applications, quick web queries.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch to Right Desktop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ctrl + Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch to Left Desktop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ctrl + Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select entire word</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opt + Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump to beginning of line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd + Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump to end of line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd + Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See next suggestion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opt + ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See previous suggestion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opt + [</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate More Results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd + Enter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open Full CoPilot Suggestions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open Chat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python: Go to Next Cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd + Opt + ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python: Go to Previous Cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd + Opt + [</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python: Extend Selection by Cell Above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd + Shift + Opt + [</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python: Extend Selection by Cell Below</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd + Shift + Alt + ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python: Move Selected Cells Up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd + ; + U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python: Move Selected Cells Down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ctrl + ; + D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python: Insert Cell Above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ctrl + ; + A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python: Insert Cell Below</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ctrl + ; + B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python: Insert Cell Below Position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ctrl + ; + S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python: Delete Selected Cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ctrl + ; + X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python: Change Cell to Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ctrl + ; + C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python: Change Cell to Markdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ctrl + ; + M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search Files by Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd + P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd + K + Cmd + S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preferences: Open Keyboard Shortcuts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show Explorer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd + Shift + E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Split Pane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go to Left Tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd + Shift + [</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View: Open Previous Editor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go to Right Tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd + Shift + ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View: Open Next Editor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go to Previous Tab in Stack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View: Open Previous Recently Used Editor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go to Next Tab in Stack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View: Open Next Recently Used Editor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open Command Palette</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd + Shift + P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show All Commands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copy Path of Current File</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd + K, P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File: Copy Path of Active File</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show File in Explorer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File: Reveal Active File in Explorer View</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search in File</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd + F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search in Files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd + Shift + F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search: Find in Files</t>
+  </si>
+  <si>
     <t xml:space="preserve">username</t>
   </si>
   <si>
@@ -73,54 +352,12 @@
     <t xml:space="preserve">user1</t>
   </si>
   <si>
-    <t xml:space="preserve">Google Sheets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show Keyboard Shortcuts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cmd + /</t>
-  </si>
-  <si>
     <t xml:space="preserve">Learning</t>
   </si>
   <si>
-    <t xml:space="preserve">See Keyboard Shortcuts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search the Menus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Opt + /</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mastered</t>
   </si>
   <si>
-    <t xml:space="preserve">Tool Finder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MacOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switch Between Open Apps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cmd + Tab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search in Files</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cmd + Shift + F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search: Find in Files</t>
-  </si>
-  <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
@@ -143,6 +380,9 @@
   </si>
   <si>
     <t xml:space="preserve">Apple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Browser</t>
   </si>
   <si>
     <t xml:space="preserve">password</t>
@@ -463,50 +703,654 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="25.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="25.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -528,7 +1372,7 @@
   </sheetPr>
   <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -549,7 +1393,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -567,25 +1411,25 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>12</v>
+        <v>105</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>14</v>
+        <v>107</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>8</v>
@@ -593,10 +1437,10 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>108</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
@@ -607,67 +1451,67 @@
         <v>18</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>108</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>108</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>108</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>29</v>
+        <v>100</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -675,10 +1519,10 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="M5" s="3" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
     </row>
     <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -753,10 +1597,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -768,7 +1612,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>111</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>7</v>
@@ -777,40 +1621,51 @@
         <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>33</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>34</v>
+        <v>113</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>35</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>37</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>38</v>
+        <v>117</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>39</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -842,36 +1697,36 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>41</v>
+        <v>121</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>42</v>
+        <v>122</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>43</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>108</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>45</v>
+        <v>125</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>15</v>
+        <v>108</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>46</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>